<commit_message>
A Functionality graphs 1
</commit_message>
<xml_diff>
--- a/3. Files/A Functionality/Sensor Characterization.xlsx
+++ b/3. Files/A Functionality/Sensor Characterization.xlsx
@@ -7,9 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Left" sheetId="1" r:id="rId1"/>
-    <sheet name="Center" sheetId="2" r:id="rId2"/>
-    <sheet name="Right" sheetId="3" r:id="rId3"/>
+    <sheet name="All three" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -61,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +75,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -113,11 +150,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,6 +176,332 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Voltage vs. Distance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'All three'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All three'!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.4933333333333336</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4133333333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9586666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2073333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'All three'!$B$7:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All three'!$F$7:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4550000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'All three'!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All three'!$F$12:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4533333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5876666666666668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9926666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7276666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="200265088"/>
+        <c:axId val="200266880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="200265088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance (in)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="200266880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="200266880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage (v)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="200265088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,501 +840,719 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>3.5</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>3.49</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>3.49</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <f>AVERAGE(C2:E2)</f>
         <v>3.4933333333333336</v>
       </c>
-      <c r="G2" s="3">
-        <f>(1023*F2)/3.3</f>
-        <v>1082.9333333333334</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="str">
+      <c r="G2" s="4">
+        <f>FLOOR((1023*F2)/3.3,3)</f>
+        <v>1080</v>
+      </c>
+      <c r="H2" s="4">
+        <f>FLOOR(G2-(5*_xlfn.STDEV.P(C2:E2)),4)</f>
+        <v>1076</v>
+      </c>
+      <c r="I2" s="4">
+        <f>CEILING(G2+(5*_xlfn.STDEV.P(C2:E2)),4)</f>
+        <v>1084</v>
+      </c>
+      <c r="J2" s="4" t="str">
         <f>DEC2HEX(G2)</f>
-        <v>43A</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+        <v>438</v>
+      </c>
+      <c r="K2" s="4" t="str">
+        <f>DEC2HEX(H2,3)</f>
+        <v>434</v>
+      </c>
+      <c r="L2" s="4" t="str">
+        <f>DEC2HEX(I2,3)</f>
+        <v>43C</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>3.42</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>3.41</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>3.41</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <f t="shared" ref="F3:F16" si="0">AVERAGE(C3:E3)</f>
         <v>3.4133333333333336</v>
       </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G16" si="1">(1023*F3)/3.3</f>
-        <v>1058.1333333333334</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="str">
-        <f t="shared" ref="J3:J16" si="2">DEC2HEX(G3)</f>
-        <v>422</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G16" si="1">FLOOR((1023*F3)/3.3,3)</f>
+        <v>1056</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H16" si="2">FLOOR(G3-(5*_xlfn.STDEV.P(C3:E3)),4)</f>
+        <v>1052</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I16" si="3">CEILING(G3+(5*_xlfn.STDEV.P(C3:E3)),4)</f>
+        <v>1060</v>
+      </c>
+      <c r="J3" s="4" t="str">
+        <f t="shared" ref="J3:J16" si="4">DEC2HEX(G3)</f>
+        <v>420</v>
+      </c>
+      <c r="K3" s="4" t="str">
+        <f t="shared" ref="K3:K16" si="5">DEC2HEX(H3,3)</f>
+        <v>41C</v>
+      </c>
+      <c r="L3" s="4" t="str">
+        <f t="shared" ref="L3:L16" si="6">DEC2HEX(I3,3)</f>
+        <v>424</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1.9750000000000001</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>1.95</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>1.9510000000000001</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>1.9586666666666666</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="4">
         <f t="shared" si="1"/>
-        <v>607.18666666666661</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3" t="str">
+        <v>606</v>
+      </c>
+      <c r="H4" s="4">
         <f t="shared" si="2"/>
-        <v>25F</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+        <v>604</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="3"/>
+        <v>608</v>
+      </c>
+      <c r="J4" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>25E</v>
+      </c>
+      <c r="K4" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>25C</v>
+      </c>
+      <c r="L4" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>260</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>1.4490000000000001</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>1.427</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>1.4139999999999999</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>1.43</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <f t="shared" si="1"/>
-        <v>443.3</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3" t="str">
+        <v>441</v>
+      </c>
+      <c r="H5" s="4">
         <f t="shared" si="2"/>
-        <v>1BB</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+        <v>440</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>444</v>
+      </c>
+      <c r="J5" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>1B9</v>
+      </c>
+      <c r="K5" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>1B8</v>
+      </c>
+      <c r="L5" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>1BC</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>1.226</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>1.216</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>1.18</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>1.2073333333333334</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="4">
         <f t="shared" si="1"/>
-        <v>374.27333333333337</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="str">
+        <v>372</v>
+      </c>
+      <c r="H6" s="4">
         <f t="shared" si="2"/>
-        <v>176</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+        <v>368</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>376</v>
+      </c>
+      <c r="J6" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>174</v>
+      </c>
+      <c r="K6" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
+      <c r="L6" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>178</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>3.5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>3.5</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>3.5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
-        <v>1085</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="str">
+        <v>1083</v>
+      </c>
+      <c r="H7" s="6">
         <f t="shared" si="2"/>
-        <v>43D</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+        <v>1080</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="3"/>
+        <v>1084</v>
+      </c>
+      <c r="J7" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>43B</v>
+      </c>
+      <c r="K7" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>438</v>
+      </c>
+      <c r="L7" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>43C</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5">
         <v>3</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>3.46</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>3.46</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>3.46</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>3.4599999999999995</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
-        <v>1072.5999999999999</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="str">
+        <v>1071</v>
+      </c>
+      <c r="H8" s="6">
         <f t="shared" si="2"/>
+        <v>1068</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="3"/>
+        <v>1072</v>
+      </c>
+      <c r="J8" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>42F</v>
+      </c>
+      <c r="K8" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>42C</v>
+      </c>
+      <c r="L8" s="6" t="str">
+        <f t="shared" si="6"/>
         <v>430</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>2.4329999999999998</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>2.4590000000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>2.4910000000000001</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>2.4609999999999999</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
-        <v>762.91000000000008</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3" t="str">
+        <v>762</v>
+      </c>
+      <c r="H9" s="6">
         <f t="shared" si="2"/>
+        <v>760</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="3"/>
+        <v>764</v>
+      </c>
+      <c r="J9" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>2FA</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="K9" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>2F8</v>
+      </c>
+      <c r="L9" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>2FC</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="5">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>1.748</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>1.7509999999999999</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>1.742</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
         <v>1.7469999999999999</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
-        <v>541.56999999999994</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3" t="str">
+        <v>540</v>
+      </c>
+      <c r="H10" s="6">
         <f t="shared" si="2"/>
-        <v>21D</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+        <v>536</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="3"/>
+        <v>544</v>
+      </c>
+      <c r="J10" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>21C</v>
+      </c>
+      <c r="K10" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>218</v>
+      </c>
+      <c r="L10" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>220</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="5">
         <v>12</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>1.4530000000000001</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="6">
         <v>1.4470000000000001</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>1.4650000000000001</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>1.4550000000000001</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
-        <v>451.05000000000007</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3" t="str">
+        <v>450</v>
+      </c>
+      <c r="H11" s="6">
         <f t="shared" si="2"/>
-        <v>1C3</v>
-      </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+        <v>448</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="3"/>
+        <v>452</v>
+      </c>
+      <c r="J11" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>1C2</v>
+      </c>
+      <c r="K11" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1C0</v>
+      </c>
+      <c r="L11" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>1C4</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="7">
         <v>1</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="8">
         <v>3.49</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="8">
         <v>3.49</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="8">
         <v>3.49</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>3.49</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="8">
         <f t="shared" si="1"/>
-        <v>1081.9000000000001</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3" t="str">
+        <v>1080</v>
+      </c>
+      <c r="H12" s="8">
         <f t="shared" si="2"/>
-        <v>439</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+        <v>1080</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" si="3"/>
+        <v>1080</v>
+      </c>
+      <c r="J12" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>438</v>
+      </c>
+      <c r="K12" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>438</v>
+      </c>
+      <c r="L12" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>438</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7">
         <v>3</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="8">
         <v>3.45</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="8">
         <v>3.46</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="8">
         <v>3.45</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="8">
         <f t="shared" si="0"/>
         <v>3.4533333333333331</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="8">
         <f t="shared" si="1"/>
-        <v>1070.5333333333333</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3" t="str">
+        <v>1068</v>
+      </c>
+      <c r="H13" s="8">
         <f t="shared" si="2"/>
-        <v>42E</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+        <v>1064</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" si="3"/>
+        <v>1072</v>
+      </c>
+      <c r="J13" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>42C</v>
+      </c>
+      <c r="K13" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>428</v>
+      </c>
+      <c r="L13" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>430</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7">
         <v>6</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="8">
         <v>2.5630000000000002</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="8">
         <v>2.6280000000000001</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="8">
         <v>2.5720000000000001</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="8">
         <f t="shared" si="0"/>
         <v>2.5876666666666668</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="8">
         <f t="shared" si="1"/>
-        <v>802.17666666666673</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="str">
+        <v>801</v>
+      </c>
+      <c r="H14" s="8">
         <f t="shared" si="2"/>
-        <v>322</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+        <v>800</v>
+      </c>
+      <c r="I14" s="8">
+        <f t="shared" si="3"/>
+        <v>804</v>
+      </c>
+      <c r="J14" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>321</v>
+      </c>
+      <c r="K14" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>320</v>
+      </c>
+      <c r="L14" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>324</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7">
         <v>9</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="8">
         <v>1.982</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="8">
         <v>1.998</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="8">
         <v>1.998</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="8">
         <f t="shared" si="0"/>
         <v>1.9926666666666666</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="8">
         <f t="shared" si="1"/>
-        <v>617.72666666666669</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3" t="str">
+        <v>615</v>
+      </c>
+      <c r="H15" s="8">
         <f t="shared" si="2"/>
-        <v>269</v>
-      </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+        <v>612</v>
+      </c>
+      <c r="I15" s="8">
+        <f t="shared" si="3"/>
+        <v>616</v>
+      </c>
+      <c r="J15" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>267</v>
+      </c>
+      <c r="K15" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>264</v>
+      </c>
+      <c r="L15" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>268</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7">
         <v>12</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="8">
         <v>1.726</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="8">
         <v>1.7230000000000001</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="8">
         <v>1.734</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="8">
         <f t="shared" si="0"/>
         <v>1.7276666666666667</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="8">
         <f t="shared" si="1"/>
-        <v>535.57666666666671</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="str">
+        <v>534</v>
+      </c>
+      <c r="H16" s="8">
         <f t="shared" si="2"/>
-        <v>217</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+        <v>532</v>
+      </c>
+      <c r="I16" s="8">
+        <f t="shared" si="3"/>
+        <v>536</v>
+      </c>
+      <c r="J16" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v>216</v>
+      </c>
+      <c r="K16" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>214</v>
+      </c>
+      <c r="L16" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>